<commit_message>
fix inezen PTAB MASTER
</commit_message>
<xml_diff>
--- a/public/cohort/fileExcel/xlsxUIT/AK PTA en onderwijsprogramma.xlsx
+++ b/public/cohort/fileExcel/xlsxUIT/AK PTA en onderwijsprogramma.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="97">
   <si>
     <t>betekenis kleuren</t>
   </si>
@@ -260,13 +260,7 @@
     <t>Overleven in Europa</t>
   </si>
   <si>
-    <t>B3, C1</t>
-  </si>
-  <si>
     <t>Opdracht met betrekking tot de eigen omgeving in combinatie met aardrijkskundige vaardigheden</t>
-  </si>
-  <si>
-    <t>A1, A2, E2, F</t>
   </si>
   <si>
     <t>PW Arm en Rijk H1en 2</t>
@@ -275,28 +269,16 @@
     <t>Arm en Rijk</t>
   </si>
   <si>
-    <t>B1, B2</t>
-  </si>
-  <si>
     <t>PW Systeem Aarde</t>
   </si>
   <si>
     <t>Katern Systeem Aarde</t>
   </si>
   <si>
-    <t>C2, C3</t>
-  </si>
-  <si>
     <t>Katern Wonen in Nederland</t>
   </si>
   <si>
-    <t>E1</t>
-  </si>
-  <si>
     <t>Katern BraziliÃ«</t>
-  </si>
-  <si>
-    <t>D1, D2</t>
   </si>
   <si>
     <t>A</t>
@@ -320,22 +302,10 @@
     <t>Katern Arm en Rijk</t>
   </si>
   <si>
-    <t>A1, B2</t>
-  </si>
-  <si>
-    <t>C1</t>
-  </si>
-  <si>
     <t>Geografische Vaardigheden gericht op katern Klimaatvraagstukken</t>
   </si>
   <si>
-    <t>A1, C2</t>
-  </si>
-  <si>
     <t>Opdracht en presentatie aan de hand van een onderzoek m.b.t. een fysisch geografisch onderdeel van klimaatvraagstukken in de eigen omgeving</t>
-  </si>
-  <si>
-    <t>C2, A2, E2</t>
   </si>
   <si>
     <t>Katern Wonen in Nederland (H1 en H2)</t>
@@ -344,16 +314,10 @@
     <t>Katern Wonen in Nederland en Globalisering</t>
   </si>
   <si>
-    <t>E1, B1</t>
-  </si>
-  <si>
     <t>Katern Zuid-Amerika</t>
   </si>
   <si>
     <t>Examenstof: Globalisering, Systeem Aarde, Zuid-Amerika, Wonen in Nederland en vaardigheden</t>
-  </si>
-  <si>
-    <t>A1, B1, C1, D1, E1</t>
   </si>
 </sst>
 </file>
@@ -1370,7 +1334,7 @@
         <v>41</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -1378,7 +1342,7 @@
         <v>1</v>
       </c>
       <c r="H6" s="28" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="I6" s="27">
         <v>1</v>
@@ -1395,9 +1359,7 @@
       <c r="O6" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="P6" s="32">
-        <v>0</v>
-      </c>
+      <c r="P6" s="32"/>
     </row>
     <row r="7" spans="1:17" customHeight="1" ht="72">
       <c r="A7" s="9" t="s">
@@ -1412,7 +1374,7 @@
         <v>1</v>
       </c>
       <c r="H7" s="28" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="I7" s="27">
         <v>2</v>
@@ -1431,9 +1393,7 @@
       <c r="O7" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="P7" s="32">
-        <v>0</v>
-      </c>
+      <c r="P7" s="32"/>
     </row>
     <row r="8" spans="1:17" customHeight="1" ht="72">
       <c r="A8" s="9" t="s">
@@ -1448,7 +1408,7 @@
         <v>2</v>
       </c>
       <c r="H8" s="28" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="I8" s="27">
         <v>2</v>
@@ -1467,9 +1427,7 @@
       <c r="O8" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="P8" s="32">
-        <v>0</v>
-      </c>
+      <c r="P8" s="32"/>
     </row>
     <row r="9" spans="1:17" customHeight="1" ht="72">
       <c r="A9" s="9" t="s">
@@ -1485,7 +1443,7 @@
         <v>3</v>
       </c>
       <c r="H9" s="28" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="I9" s="27">
         <v>3</v>
@@ -1504,9 +1462,7 @@
       <c r="O9" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="P9" s="32" t="s">
-        <v>79</v>
-      </c>
+      <c r="P9" s="32"/>
     </row>
     <row r="10" spans="1:17" customHeight="1" ht="72">
       <c r="A10" s="9" t="s">
@@ -1514,7 +1470,7 @@
       </c>
       <c r="B10" s="6">
         <f>NOW()</f>
-        <v>44334.63337963</v>
+        <v>44335.8084375</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -1522,7 +1478,7 @@
         <v>4</v>
       </c>
       <c r="H10" s="28" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="I10" s="27">
         <v>2</v>
@@ -1541,9 +1497,7 @@
       <c r="O10" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="P10" s="32">
-        <v>0</v>
-      </c>
+      <c r="P10" s="32"/>
     </row>
     <row r="11" spans="1:17" customHeight="1" ht="72">
       <c r="A11" s="9" t="s">
@@ -1559,7 +1513,7 @@
         <v>4</v>
       </c>
       <c r="H11" s="28" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="I11" s="27">
         <v>3</v>
@@ -1580,9 +1534,7 @@
       <c r="O11" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="P11" s="32" t="s">
-        <v>97</v>
-      </c>
+      <c r="P11" s="32"/>
     </row>
     <row r="12" spans="1:17">
       <c r="A12" s="9" t="s">
@@ -2284,7 +2236,7 @@
         <v>41</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -2398,7 +2350,7 @@
       </c>
       <c r="B10" s="6">
         <f>NOW()</f>
-        <v>44334.63337963</v>
+        <v>44335.8084375</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -2553,7 +2505,7 @@
         <v>1</v>
       </c>
       <c r="H18" s="28" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="I18" s="27">
         <v>1</v>
@@ -2570,9 +2522,7 @@
       <c r="O18" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="P18" s="32">
-        <v>0</v>
-      </c>
+      <c r="P18" s="32"/>
     </row>
     <row r="19" spans="1:17" customHeight="1" ht="72">
       <c r="D19" s="2"/>
@@ -2581,7 +2531,7 @@
         <v>1</v>
       </c>
       <c r="H19" s="28" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I19" s="27">
         <v>2</v>
@@ -2600,9 +2550,7 @@
       <c r="O19" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="P19" s="32">
-        <v>0</v>
-      </c>
+      <c r="P19" s="32"/>
     </row>
     <row r="20" spans="1:17" customHeight="1" ht="72">
       <c r="D20" s="2"/>
@@ -2611,7 +2559,7 @@
         <v>2</v>
       </c>
       <c r="H20" s="28" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I20" s="27">
         <v>3</v>
@@ -2632,9 +2580,7 @@
       <c r="O20" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="P20" s="32" t="s">
-        <v>98</v>
-      </c>
+      <c r="P20" s="32"/>
     </row>
     <row r="21" spans="1:17" customHeight="1" ht="72">
       <c r="D21" s="2"/>
@@ -2643,7 +2589,7 @@
         <v>3</v>
       </c>
       <c r="H21" s="28" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="I21" s="27">
         <v>3</v>
@@ -2664,9 +2610,7 @@
       <c r="O21" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="P21" s="32" t="s">
-        <v>100</v>
-      </c>
+      <c r="P21" s="32"/>
     </row>
     <row r="22" spans="1:17" customHeight="1" ht="72">
       <c r="D22" s="2"/>
@@ -2675,7 +2619,7 @@
         <v>3</v>
       </c>
       <c r="H22" s="28" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="I22" s="27">
         <v>3</v>
@@ -2694,9 +2638,7 @@
       <c r="O22" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="P22" s="32" t="s">
-        <v>102</v>
-      </c>
+      <c r="P22" s="32"/>
     </row>
     <row r="23" spans="1:17" customHeight="1" ht="72">
       <c r="D23" s="2"/>
@@ -2705,7 +2647,7 @@
         <v>4</v>
       </c>
       <c r="H23" s="28" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="I23" s="27">
         <v>3</v>
@@ -2726,9 +2668,7 @@
       <c r="O23" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="P23" s="32" t="s">
-        <v>87</v>
-      </c>
+      <c r="P23" s="32"/>
     </row>
     <row r="25" spans="1:17">
       <c r="C25" s="9" t="s">
@@ -3202,7 +3142,7 @@
         <v>41</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
@@ -3316,7 +3256,7 @@
       </c>
       <c r="B10" s="6">
         <f>NOW()</f>
-        <v>44334.63337963</v>
+        <v>44335.8084375</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -3676,7 +3616,7 @@
         <v>1</v>
       </c>
       <c r="H30" s="28" t="s">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="I30" s="27"/>
       <c r="J30" s="29" t="s">
@@ -3695,9 +3635,7 @@
       <c r="O30" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="P30" s="32" t="s">
-        <v>105</v>
-      </c>
+      <c r="P30" s="32"/>
     </row>
     <row r="31" spans="1:17" customHeight="1" ht="72">
       <c r="D31" s="2"/>
@@ -3706,7 +3644,7 @@
         <v>2</v>
       </c>
       <c r="H31" s="28" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="I31" s="27"/>
       <c r="J31" s="29" t="s">
@@ -3725,9 +3663,7 @@
       <c r="O31" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="P31" s="32" t="s">
-        <v>89</v>
-      </c>
+      <c r="P31" s="32"/>
     </row>
     <row r="32" spans="1:17" customHeight="1" ht="72">
       <c r="D32" s="2"/>
@@ -3736,7 +3672,7 @@
         <v>3</v>
       </c>
       <c r="H32" s="28" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="I32" s="27"/>
       <c r="J32" s="29" t="s">
@@ -3755,9 +3691,7 @@
       <c r="O32" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="P32" s="32" t="s">
-        <v>108</v>
-      </c>
+      <c r="P32" s="32"/>
     </row>
     <row r="33" spans="1:17" customHeight="1" ht="72">
       <c r="D33" s="2"/>
@@ -4196,7 +4130,7 @@
       </c>
       <c r="B10" s="6">
         <f>NOW()</f>
-        <v>44334.63337963</v>
+        <v>44335.8084375</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -5151,7 +5085,7 @@
       </c>
       <c r="B10" s="6">
         <f>NOW()</f>
-        <v>44334.63337963</v>
+        <v>44335.8084375</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -5967,7 +5901,7 @@
       </c>
       <c r="B10" s="6">
         <f>NOW()</f>
-        <v>44334.63337963</v>
+        <v>44335.8084375</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -6783,7 +6717,7 @@
       </c>
       <c r="B10" s="6">
         <f>NOW()</f>
-        <v>44334.63337963</v>
+        <v>44335.8084375</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -7522,9 +7456,7 @@
       <c r="O6" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="P6" s="32">
-        <v>0</v>
-      </c>
+      <c r="P6" s="32"/>
     </row>
     <row r="7" spans="1:17" customHeight="1" ht="72">
       <c r="A7" s="9" t="s">
@@ -7560,9 +7492,7 @@
       <c r="O7" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="P7" s="32" t="s">
-        <v>77</v>
-      </c>
+      <c r="P7" s="32"/>
     </row>
     <row r="8" spans="1:17" customHeight="1" ht="72">
       <c r="A8" s="9" t="s">
@@ -7577,7 +7507,7 @@
         <v>2</v>
       </c>
       <c r="H8" s="28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I8" s="27">
         <v>3</v>
@@ -7596,9 +7526,7 @@
       <c r="O8" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="P8" s="32" t="s">
-        <v>79</v>
-      </c>
+      <c r="P8" s="32"/>
     </row>
     <row r="9" spans="1:17" customHeight="1" ht="72">
       <c r="A9" s="9" t="s">
@@ -7614,7 +7542,7 @@
         <v>2</v>
       </c>
       <c r="H9" s="28" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="I9" s="27">
         <v>2</v>
@@ -7633,9 +7561,7 @@
       <c r="O9" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="P9" s="32">
-        <v>0</v>
-      </c>
+      <c r="P9" s="32"/>
     </row>
     <row r="10" spans="1:17" customHeight="1" ht="72">
       <c r="A10" s="9" t="s">
@@ -7643,7 +7569,7 @@
       </c>
       <c r="B10" s="6">
         <f>NOW()</f>
-        <v>44334.63337963</v>
+        <v>44335.8084375</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -7651,7 +7577,7 @@
         <v>3</v>
       </c>
       <c r="H10" s="28" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I10" s="27">
         <v>3</v>
@@ -7672,9 +7598,7 @@
       <c r="O10" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="P10" s="32" t="s">
-        <v>82</v>
-      </c>
+      <c r="P10" s="32"/>
     </row>
     <row r="11" spans="1:17" customHeight="1" ht="72">
       <c r="A11" s="9" t="s">
@@ -7690,7 +7614,7 @@
         <v>4</v>
       </c>
       <c r="H11" s="28" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="I11" s="27">
         <v>2</v>
@@ -7709,9 +7633,7 @@
       <c r="O11" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="P11" s="32">
-        <v>0</v>
-      </c>
+      <c r="P11" s="32"/>
     </row>
     <row r="12" spans="1:17">
       <c r="A12" s="9" t="s">
@@ -8527,7 +8449,7 @@
       </c>
       <c r="B10" s="6">
         <f>NOW()</f>
-        <v>44334.63337963</v>
+        <v>44335.8084375</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -8682,7 +8604,7 @@
         <v>1</v>
       </c>
       <c r="H18" s="28" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="I18" s="27"/>
       <c r="J18" s="29" t="s">
@@ -8701,9 +8623,7 @@
       <c r="O18" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="P18" s="32" t="s">
-        <v>85</v>
-      </c>
+      <c r="P18" s="32"/>
     </row>
     <row r="19" spans="1:17" customHeight="1" ht="72">
       <c r="D19" s="2"/>
@@ -8712,7 +8632,7 @@
         <v>2</v>
       </c>
       <c r="H19" s="28" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="I19" s="27"/>
       <c r="J19" s="29" t="s">
@@ -8731,9 +8651,7 @@
       <c r="O19" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="P19" s="32" t="s">
-        <v>87</v>
-      </c>
+      <c r="P19" s="32"/>
     </row>
     <row r="20" spans="1:17" customHeight="1" ht="72">
       <c r="D20" s="2"/>
@@ -8742,7 +8660,7 @@
         <v>3</v>
       </c>
       <c r="H20" s="28" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="I20" s="27"/>
       <c r="J20" s="29" t="s">
@@ -8761,9 +8679,7 @@
       <c r="O20" s="31" t="s">
         <v>11</v>
       </c>
-      <c r="P20" s="32" t="s">
-        <v>89</v>
-      </c>
+      <c r="P20" s="32"/>
     </row>
     <row r="21" spans="1:17" customHeight="1" ht="72">
       <c r="D21" s="2"/>
@@ -9407,7 +9323,7 @@
       </c>
       <c r="B10" s="6">
         <f>NOW()</f>
-        <v>44334.63337963</v>
+        <v>44335.8084375</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>

</xml_diff>